<commit_message>
Added images for the buttons int ExcelTest
</commit_message>
<xml_diff>
--- a/ExcelTest/ExcelTest/bin/Debug/test.xlsx
+++ b/ExcelTest/ExcelTest/bin/Debug/test.xlsx
@@ -693,7 +693,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -704,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1551682</v>
+        <v>155168</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1555533</v>
+        <v>155553</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2526290</v>
+        <v>252629</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2162899</v>
+        <v>216289</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2606758</v>
+        <v>260675</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>140020</v>
+        <v>14002</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2607060</v>
+        <v>260706</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>3095076</v>
+        <v>309507</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>1162408</v>
+        <v>116240</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>8</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2509618</v>
+        <v>250961</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>775280</v>
+        <v>77528</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1347757</v>
+        <v>134775</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2876802</v>
+        <v>287680</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2359449</v>
+        <v>235944</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2828200</v>
+        <v>282820</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2792494</v>
+        <v>279249</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2668736</v>
+        <v>266873</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2628234</v>
+        <v>262823</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>155620</v>
+        <v>15562</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1296043</v>
+        <v>129604</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>2277616</v>
+        <v>227761</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1171407</v>
+        <v>117140</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1555763</v>
+        <v>155576</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>767180</v>
+        <v>76718</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>2604009</v>
+        <v>260400</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>2854686</v>
+        <v>285468</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>2828200</v>
+        <v>282820</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>15</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>3070521</v>
+        <v>307052</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>101008</v>
+        <v>10100</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>29</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>633194</v>
+        <v>63319</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>31</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>2798120</v>
+        <v>279812</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>32</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>3188837</v>
+        <v>318883</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>33</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>123688</v>
+        <v>12368</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>34</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>239698</v>
+        <v>23969</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2879870</v>
+        <v>287987</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>36</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>36713</v>
+        <v>3671</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>37</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>2839089</v>
+        <v>283908</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>38</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>1891159</v>
+        <v>189115</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>39</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>774807</v>
+        <v>77480</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>40</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>142036</v>
+        <v>14203</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>41</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>2868292</v>
+        <v>286829</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>42</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>2782159</v>
+        <v>278215</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>43</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>2627401</v>
+        <v>262740</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>44</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>3179264</v>
+        <v>317926</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>45</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>2724481</v>
+        <v>272448</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>46</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>2828200</v>
+        <v>282820</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>15</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>3221983</v>
+        <v>322198</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>47</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>1394366</v>
+        <v>139436</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>48</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>305679</v>
+        <v>30567</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>49</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>2759551</v>
+        <v>275955</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>50</v>
@@ -1902,7 +1902,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>2759551</v>
+        <v>275955</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>50</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>3139862</v>
+        <v>313986</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>51</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>26028</v>
+        <v>2602</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>52</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>2968390</v>
+        <v>296839</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>53</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>778768</v>
+        <v>77876</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>54</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>1872630</v>
+        <v>187263</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>56</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>52103</v>
+        <v>5210</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>57</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>2376531</v>
+        <v>237653</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>58</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>2898399</v>
+        <v>289839</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>59</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>2577040</v>
+        <v>257704</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>60</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>2154569</v>
+        <v>215456</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>61</v>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>1163170</v>
+        <v>116317</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>62</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>640521</v>
+        <v>64052</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>63</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>2969700</v>
+        <v>296970</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>64</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>2262603</v>
+        <v>226260</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>65</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>2464459</v>
+        <v>246445</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>66</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>2564267</v>
+        <v>256426</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>67</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>1209009</v>
+        <v>120900</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>68</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>2719400</v>
+        <v>271940</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>69</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1409949</v>
+        <v>140994</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>70</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>2576218</v>
+        <v>257621</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>71</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1248771</v>
+        <v>124877</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>72</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1565069</v>
+        <v>156506</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>73</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>2453220</v>
+        <v>245322</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>74</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>317560</v>
+        <v>31756</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>75</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>2798120</v>
+        <v>279812</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>32</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>1550040</v>
+        <v>155004</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>76</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>95383</v>
+        <v>9538</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>77</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>3122608</v>
+        <v>312260</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>78</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>2859650</v>
+        <v>285965</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>79</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>750155</v>
+        <v>75015</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>80</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>3119351</v>
+        <v>311935</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>81</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>3132363</v>
+        <v>313236</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>82</v>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>2359449</v>
+        <v>235944</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>14</v>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>535451</v>
+        <v>53545</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>83</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>3114804</v>
+        <v>311480</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>84</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1392580</v>
+        <v>139258</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>85</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>535451</v>
+        <v>53545</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>83</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>2948000</v>
+        <v>294800</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>86</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>2118088</v>
+        <v>211808</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>87</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>3201302</v>
+        <v>320130</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>88</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>1394366</v>
+        <v>139436</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>48</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>2165277</v>
+        <v>216527</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>89</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>324197</v>
+        <v>32419</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>90</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>2493142</v>
+        <v>249314</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>91</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>532033</v>
+        <v>53203</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Fixed borders problem (kind of)
</commit_message>
<xml_diff>
--- a/ExcelTest/ExcelTest/bin/Debug/test.xlsx
+++ b/ExcelTest/ExcelTest/bin/Debug/test.xlsx
@@ -304,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,61 +313,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -389,46 +356,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,2312 +658,2312 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>15516820</v>
+        <v>155168</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1">
         <v>60</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="1">
         <v>164.4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="1">
         <v>69110710</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="1">
         <v>131</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>15555330</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="2">
+        <v>155553</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>6</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="2">
         <v>137.76</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="2">
         <v>41050410</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="2">
         <v>131</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>25262905</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="2">
+        <v>252629</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
         <v>12</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="2">
         <v>125.88</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="2">
         <v>50060000</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>21628999</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="2">
+        <v>216289</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="2">
         <v>18</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="2">
         <v>42260000</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="2">
         <v>188</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>26067583</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="2">
+        <v>260675</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>8</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="2">
         <v>41.84</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="2">
         <v>51120420</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="2">
         <v>12</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>1400204</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="2">
+        <v>14002</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>67</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="2">
         <v>381.9</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="2">
         <v>18020000</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="2">
         <v>425</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>26070600</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="2">
+        <v>260706</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>8</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="2">
         <v>49.44</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="2">
         <v>51070540</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="2">
         <v>50</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>30950760</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="2">
+        <v>309507</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>48</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="2">
         <v>32.64</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="2">
         <v>59120520</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="2">
         <v>118</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>11624085</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="2">
+        <v>116240</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
         <v>240</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="2">
         <v>315.36</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="2">
         <v>58100000</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="2">
         <v>400</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>25096186</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="2">
+        <v>250961</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2">
         <v>60.4</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="2">
         <v>67010210</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="2">
         <v>97</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>7752803</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="2">
+        <v>77528</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>100</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="2">
         <v>254</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="2">
         <v>84110920</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="2">
         <v>61</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>13477576</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="2">
+        <v>134775</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <v>40</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="3">
         <v>1123.2</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="2">
         <v>71180610</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="2">
         <v>219</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>28768025</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="2">
+        <v>287680</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>512</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="3">
         <v>1689.6</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="2">
         <v>73100520</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="2">
         <v>526</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>23594490</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="2">
+        <v>235944</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7">
-        <v>10</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
         <v>44</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="2">
         <v>25400000</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="4">
         <v>3282</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>28282009</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="2">
+        <v>282820</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>40</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="2">
         <v>336.4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="2">
         <v>73140420</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="2">
         <v>450</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>27924948</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="2">
+        <v>279249</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7">
-        <v>10</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2">
         <v>22.9</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="2">
         <v>45190230</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="2">
         <v>25</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>26687363</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="2">
+        <v>266873</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7">
-        <v>10</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
         <v>42</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="2">
         <v>47110330</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="2">
         <v>289</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>26282347</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="2">
+        <v>262823</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
         <v>96</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="3">
         <v>1138.56</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="2">
         <v>73110410</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="2">
         <v>74</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>1556202</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="2">
+        <v>15562</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
         <v>30</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="2">
         <v>80.099999999999994</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="2">
         <v>23190000</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="2">
         <v>357</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>12960431</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="2">
+        <v>129604</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
         <v>80</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="2">
         <v>472.8</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="2">
         <v>64050000</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="2">
         <v>475</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>22776160</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="2">
+        <v>227761</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
         <v>120</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="2">
         <v>579.6</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="2">
         <v>19270000</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="4">
         <v>2698</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>11714078</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="2">
+        <v>117140</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
         <v>400</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="3">
         <v>2544</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="2">
         <v>3010300</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="4">
         <v>2095</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>15557635</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="2">
+        <v>155576</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
         <v>5</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="2">
         <v>93.95</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="2">
         <v>32040310</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="2">
         <v>0</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>7671803</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="2">
+        <v>76718</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2">
         <v>50</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="2">
         <v>127</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="2">
         <v>68051620</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="2">
         <v>41</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>26040093</v>
-      </c>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="2">
+        <v>260400</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
         <v>4</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="2">
         <v>14.72</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="2">
         <v>63040160</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="2">
         <v>14</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>28546862</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="2">
+        <v>285468</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
         <v>40</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="2">
         <v>117.2</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="2">
         <v>61020430</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="2">
         <v>668</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>28282009</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="2">
+        <v>282820</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
         <v>100</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="2">
         <v>841</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="2">
         <v>53070340</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="2">
         <v>41</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>30705210</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="2">
+        <v>307052</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7">
-        <v>10</v>
-      </c>
-      <c r="E28" s="7">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2">
         <v>90.2</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="2">
         <v>27040460</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="2">
         <v>7</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>1010087</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="2">
+        <v>10100</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2">
         <v>180</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="2">
         <v>502.2</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="2">
         <v>5110000</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="4">
         <v>2902</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>6331940</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="2">
+        <v>63319</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
         <v>80</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="2">
         <v>224</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="2">
         <v>15010130</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="4">
         <v>5205</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>27981202</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="2">
+        <v>279812</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="7">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2">
         <v>24</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="2">
         <v>132.96</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="2">
         <v>45030660</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="2">
         <v>58</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>31888370</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="2">
+        <v>318883</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2">
         <v>12</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="2">
         <v>39.119999999999997</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="2">
         <v>40050660</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="2">
         <v>18</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>1236880</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="2">
+        <v>12368</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2">
         <v>300</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="3">
         <v>1005</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="2">
         <v>12030320</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="4">
         <v>1049</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>2396982</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="2">
+        <v>23969</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2">
         <v>900</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="3">
         <v>3087</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="2">
         <v>1210000</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="4">
         <v>4265</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>28798701</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="2">
+        <v>287987</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2">
         <v>52</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="2">
         <v>377.52</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="2">
         <v>15050240</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="2">
         <v>77</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>367137</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="2">
+        <v>3671</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2">
         <v>8</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="2">
         <v>191.92</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="2">
         <v>42010510</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="2">
         <v>29</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>28390897</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="2">
+        <v>283908</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2">
         <v>7</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="2">
         <v>66.989999999999995</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="2">
         <v>60040110</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="2">
         <v>34</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>18911592</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="2">
+        <v>189115</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2">
         <v>72</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="2">
         <v>354.24</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="2">
         <v>41001200</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="2">
         <v>427</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>7748078</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="2">
+        <v>77480</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2">
         <v>20</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="2">
         <v>50.8</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="2">
         <v>63111100</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="2">
         <v>19</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>1420365</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="2">
+        <v>14203</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2">
         <v>180</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="3">
         <v>1053</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="2">
         <v>13030110</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="2">
         <v>568</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>28682921</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="2">
+        <v>286829</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2">
         <v>5</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="2">
         <v>166.1</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="2">
         <v>47050430</v>
       </c>
-      <c r="G41" s="7">
-        <v>10</v>
-      </c>
-      <c r="H41" s="8" t="s">
+      <c r="G41" s="2">
+        <v>10</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>27821591</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="2">
+        <v>278215</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2">
         <v>5</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="2">
         <v>14.5</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="2">
         <v>56060160</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="2">
         <v>5</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>26274017</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="A43" s="2">
+        <v>262740</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="7">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2">
         <v>60</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="2">
         <v>909</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="2">
         <v>42020630</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="2">
         <v>965</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>31792641</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="2">
+        <v>317926</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2">
         <v>17</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="2">
         <v>170.17</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="2">
         <v>45040560</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="2">
         <v>100</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>27244811</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="2">
+        <v>272448</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="7">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2">
         <v>12</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="2">
         <v>37.799999999999997</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="2">
         <v>57020140</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="2">
         <v>28</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
-        <v>28282009</v>
-      </c>
-      <c r="B46" s="5" t="s">
+      <c r="A46" s="2">
+        <v>282820</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2">
         <v>100</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="2">
         <v>841</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="2">
         <v>12060240</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="2">
         <v>116</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>32219837</v>
-      </c>
-      <c r="B47" s="5" t="s">
+      <c r="A47" s="2">
+        <v>322198</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2">
         <v>48</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="2">
         <v>272.16000000000003</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="7">
+      <c r="F47" s="2"/>
+      <c r="G47" s="2">
         <v>0</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <v>13943660</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="2">
+        <v>139436</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="7">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2">
         <v>12</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="2">
         <v>83.4</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="2">
         <v>48060520</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="2">
         <v>0</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
-        <v>3056797</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="A49" s="2">
+        <v>30567</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2">
         <v>240</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="2">
         <v>268.8</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="2">
         <v>41010410</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="2">
         <v>318</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>27595516</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="A50" s="2">
+        <v>275955</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="7">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2">
         <v>34</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="2">
         <v>121.72</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="2">
         <v>23070110</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="4">
         <v>1226</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="H50" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <v>27595516</v>
-      </c>
-      <c r="B51" s="5" t="s">
+      <c r="A51" s="2">
+        <v>275955</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="7">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2">
         <v>36</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="2">
         <v>128.88</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="2">
         <v>23070110</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="4">
         <v>1226</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
-        <v>31398625</v>
-      </c>
-      <c r="B52" s="5" t="s">
+      <c r="A52" s="2">
+        <v>313986</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="7">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2">
         <v>42</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="2">
         <v>205.8</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="2">
         <v>15070350</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G52" s="2">
         <v>159</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
-        <v>260280</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="A53" s="2">
+        <v>2602</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2">
         <v>16</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="2">
         <v>36.96</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="2">
         <v>67020450</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G53" s="2">
         <v>976</v>
       </c>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
-        <v>29683905</v>
-      </c>
-      <c r="B54" s="5" t="s">
+      <c r="A54" s="2">
+        <v>296839</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7">
-        <v>10</v>
-      </c>
-      <c r="E54" s="7">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2">
+        <v>10</v>
+      </c>
+      <c r="E54" s="2">
         <v>159.80000000000001</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F54" s="2">
         <v>16060610</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G54" s="2">
         <v>73</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="H54" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
-        <v>7787687</v>
-      </c>
-      <c r="B55" s="5" t="s">
+      <c r="A55" s="2">
+        <v>77876</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2">
         <v>80</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="2">
         <v>492</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="2">
         <v>14102100</v>
       </c>
-      <c r="G55" s="7">
+      <c r="G55" s="2">
         <v>296</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
-        <v>18726305</v>
-      </c>
-      <c r="B56" s="5" t="s">
+      <c r="A56" s="2">
+        <v>187263</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="7">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2">
         <v>30</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="2">
         <v>35.4</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F56" s="2">
         <v>46025000</v>
       </c>
-      <c r="G56" s="7">
+      <c r="G56" s="2">
         <v>441</v>
       </c>
-      <c r="H56" s="8" t="s">
+      <c r="H56" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>521035</v>
-      </c>
-      <c r="B57" s="5" t="s">
+      <c r="A57" s="2">
+        <v>5210</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="7">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2">
         <v>30</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="2">
         <v>66.900000000000006</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="2">
         <v>5270000</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="4">
         <v>3816</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="H57" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
-        <v>23765312</v>
-      </c>
-      <c r="B58" s="5" t="s">
+      <c r="A58" s="2">
+        <v>237653</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="7">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2">
         <v>14</v>
       </c>
-      <c r="E58" s="7">
+      <c r="E58" s="2">
         <v>153.44</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F58" s="2">
         <v>60103400</v>
       </c>
-      <c r="G58" s="7">
+      <c r="G58" s="2">
         <v>18</v>
       </c>
-      <c r="H58" s="8" t="s">
+      <c r="H58" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
-        <v>28983999</v>
-      </c>
-      <c r="B59" s="5" t="s">
+      <c r="A59" s="2">
+        <v>289839</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="7">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2">
         <v>70</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="2">
         <v>449.4</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="2">
         <v>30033500</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="2">
         <v>122</v>
       </c>
-      <c r="H59" s="8" t="s">
+      <c r="H59" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>25770406</v>
-      </c>
-      <c r="B60" s="5" t="s">
+      <c r="A60" s="2">
+        <v>257704</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2">
         <v>1</v>
       </c>
-      <c r="E60" s="12">
+      <c r="E60" s="3">
         <v>1589.58</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="2">
         <v>84025400</v>
       </c>
-      <c r="G60" s="7">
+      <c r="G60" s="2">
         <v>7</v>
       </c>
-      <c r="H60" s="8" t="s">
+      <c r="H60" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>21545693</v>
-      </c>
-      <c r="B61" s="5" t="s">
+      <c r="A61" s="2">
+        <v>215456</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="7">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2">
         <v>60</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61" s="2">
         <v>692.4</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F61" s="2">
         <v>82012400</v>
       </c>
-      <c r="G61" s="7">
+      <c r="G61" s="2">
         <v>0</v>
       </c>
-      <c r="H61" s="8" t="s">
+      <c r="H61" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
-        <v>11631702</v>
-      </c>
-      <c r="B62" s="5" t="s">
+      <c r="A62" s="2">
+        <v>116317</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="7">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2">
         <v>48</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="2">
         <v>58.08</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="2">
         <v>58095100</v>
       </c>
-      <c r="G62" s="7">
+      <c r="G62" s="2">
         <v>151</v>
       </c>
-      <c r="H62" s="8" t="s">
+      <c r="H62" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
-        <v>6405212</v>
-      </c>
-      <c r="B63" s="5" t="s">
+      <c r="A63" s="2">
+        <v>64052</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="7">
-        <v>10</v>
-      </c>
-      <c r="E63" s="7">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2">
+        <v>10</v>
+      </c>
+      <c r="E63" s="2">
         <v>90.8</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="2">
         <v>19033300</v>
       </c>
-      <c r="G63" s="7">
+      <c r="G63" s="2">
         <v>38</v>
       </c>
-      <c r="H63" s="8" t="s">
+      <c r="H63" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
-        <v>29697008</v>
-      </c>
-      <c r="B64" s="5" t="s">
+      <c r="A64" s="2">
+        <v>296970</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="7">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2">
         <v>20</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64" s="2">
         <v>273.8</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="2">
         <v>67033200</v>
       </c>
-      <c r="G64" s="7">
+      <c r="G64" s="2">
         <v>562</v>
       </c>
-      <c r="H64" s="8" t="s">
+      <c r="H64" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <v>22626034</v>
-      </c>
-      <c r="B65" s="5" t="s">
+      <c r="A65" s="2">
+        <v>226260</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="7">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2">
         <v>54</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="2">
         <v>41.58</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="2">
         <v>58016100</v>
       </c>
-      <c r="G65" s="7">
+      <c r="G65" s="2">
         <v>41</v>
       </c>
-      <c r="H65" s="8" t="s">
+      <c r="H65" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
-        <v>24644591</v>
-      </c>
-      <c r="B66" s="5" t="s">
+      <c r="A66" s="2">
+        <v>246445</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="7">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2">
         <v>30</v>
       </c>
-      <c r="E66" s="7">
+      <c r="E66" s="2">
         <v>145.5</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F66" s="2">
         <v>25021300</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="4">
         <v>1098</v>
       </c>
-      <c r="H66" s="8" t="s">
+      <c r="H66" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
-        <v>25642677</v>
-      </c>
-      <c r="B67" s="5" t="s">
+      <c r="A67" s="2">
+        <v>256426</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="7">
-        <v>10</v>
-      </c>
-      <c r="E67" s="7">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2">
+        <v>10</v>
+      </c>
+      <c r="E67" s="2">
         <v>114.2</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="2">
         <v>32074600</v>
       </c>
-      <c r="G67" s="7">
+      <c r="G67" s="2">
         <v>115</v>
       </c>
-      <c r="H67" s="8" t="s">
+      <c r="H67" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
-        <v>12090094</v>
-      </c>
-      <c r="B68" s="5" t="s">
+      <c r="A68" s="2">
+        <v>120900</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="7">
+      <c r="C68" s="2"/>
+      <c r="D68" s="2">
         <v>18</v>
       </c>
-      <c r="E68" s="7">
+      <c r="E68" s="2">
         <v>88.56</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F68" s="2">
         <v>60042300</v>
       </c>
-      <c r="G68" s="7">
+      <c r="G68" s="2">
         <v>322</v>
       </c>
-      <c r="H68" s="8" t="s">
+      <c r="H68" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
-        <v>27194007</v>
-      </c>
-      <c r="B69" s="5" t="s">
+      <c r="A69" s="2">
+        <v>271940</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="7">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2">
         <v>100</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="2">
         <v>450</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="2">
         <v>69034200</v>
       </c>
-      <c r="G69" s="7">
+      <c r="G69" s="2">
         <v>378</v>
       </c>
-      <c r="H69" s="8" t="s">
+      <c r="H69" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
-        <v>14099490</v>
-      </c>
-      <c r="B70" s="5" t="s">
+      <c r="A70" s="2">
+        <v>140994</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="7">
-        <v>10</v>
-      </c>
-      <c r="E70" s="7">
+      <c r="C70" s="2"/>
+      <c r="D70" s="2">
+        <v>10</v>
+      </c>
+      <c r="E70" s="2">
         <v>42.5</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F70" s="2">
         <v>42025200</v>
       </c>
-      <c r="G70" s="7">
+      <c r="G70" s="2">
         <v>2</v>
       </c>
-      <c r="H70" s="8" t="s">
+      <c r="H70" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>25762186</v>
-      </c>
-      <c r="B71" s="5" t="s">
+      <c r="A71" s="2">
+        <v>257621</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="7">
+      <c r="C71" s="2"/>
+      <c r="D71" s="2">
         <v>15</v>
       </c>
-      <c r="E71" s="7">
+      <c r="E71" s="2">
         <v>40.5</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F71" s="2">
         <v>51075300</v>
       </c>
-      <c r="G71" s="7">
+      <c r="G71" s="2">
         <v>33</v>
       </c>
-      <c r="H71" s="8" t="s">
+      <c r="H71" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
-        <v>12487710</v>
-      </c>
-      <c r="B72" s="5" t="s">
+      <c r="A72" s="2">
+        <v>124877</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="7">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2">
         <v>36</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="2">
         <v>183.24</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F72" s="2">
         <v>35111200</v>
       </c>
-      <c r="G72" s="7">
+      <c r="G72" s="2">
         <v>51</v>
       </c>
-      <c r="H72" s="8" t="s">
+      <c r="H72" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
-        <v>15650694</v>
-      </c>
-      <c r="B73" s="5" t="s">
+      <c r="A73" s="2">
+        <v>156506</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="7">
+      <c r="C73" s="2"/>
+      <c r="D73" s="2">
         <v>5</v>
       </c>
-      <c r="E73" s="7">
+      <c r="E73" s="2">
         <v>36.15</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="2">
         <v>63095500</v>
       </c>
-      <c r="G73" s="7">
+      <c r="G73" s="2">
         <v>135</v>
       </c>
-      <c r="H73" s="8" t="s">
+      <c r="H73" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
-        <v>24532202</v>
-      </c>
-      <c r="B74" s="5" t="s">
+      <c r="A74" s="2">
+        <v>245322</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="7">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2">
         <v>100</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="2">
         <v>220</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="2">
         <v>65085300</v>
       </c>
-      <c r="G74" s="7">
+      <c r="G74" s="2">
         <v>136</v>
       </c>
-      <c r="H74" s="8" t="s">
+      <c r="H74" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
-        <v>3175600</v>
-      </c>
-      <c r="B75" s="5" t="s">
+      <c r="A75" s="2">
+        <v>31756</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="7">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2">
         <v>40</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E75" s="2">
         <v>82</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F75" s="2">
         <v>8012000</v>
       </c>
-      <c r="G75" s="13">
+      <c r="G75" s="4">
         <v>3349</v>
       </c>
-      <c r="H75" s="8" t="s">
+      <c r="H75" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
-        <v>27981202</v>
-      </c>
-      <c r="B76" s="5" t="s">
+      <c r="A76" s="2">
+        <v>279812</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="7">
+      <c r="C76" s="2"/>
+      <c r="D76" s="2">
         <v>24</v>
       </c>
-      <c r="E76" s="7">
+      <c r="E76" s="2">
         <v>132.96</v>
       </c>
-      <c r="F76" s="7">
+      <c r="F76" s="2">
         <v>33035200</v>
       </c>
-      <c r="G76" s="7">
+      <c r="G76" s="2">
         <v>49</v>
       </c>
-      <c r="H76" s="8" t="s">
+      <c r="H76" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <v>15500405</v>
-      </c>
-      <c r="B77" s="5" t="s">
+      <c r="A77" s="2">
+        <v>155004</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="7">
+      <c r="C77" s="2"/>
+      <c r="D77" s="2">
         <v>18</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E77" s="2">
         <v>181.26</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="2">
         <v>40026100</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G77" s="2">
         <v>378</v>
       </c>
-      <c r="H77" s="8" t="s">
+      <c r="H77" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
-        <v>953830</v>
-      </c>
-      <c r="B78" s="5" t="s">
+      <c r="A78" s="2">
+        <v>9538</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="7">
+      <c r="C78" s="2"/>
+      <c r="D78" s="2">
         <v>350</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E78" s="2">
         <v>402.5</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F78" s="2">
         <v>39012100</v>
       </c>
-      <c r="G78" s="13">
+      <c r="G78" s="4">
         <v>7049</v>
       </c>
-      <c r="H78" s="8" t="s">
+      <c r="H78" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
-        <v>31226083</v>
-      </c>
-      <c r="B79" s="5" t="s">
+      <c r="A79" s="2">
+        <v>312260</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="7">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2">
         <v>15</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E79" s="2">
         <v>114.3</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F79" s="2">
         <v>14081400</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G79" s="2">
         <v>71</v>
       </c>
-      <c r="H79" s="8" t="s">
+      <c r="H79" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
-        <v>28596506</v>
-      </c>
-      <c r="B80" s="5" t="s">
+      <c r="A80" s="2">
+        <v>285965</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="7">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2">
         <v>12</v>
       </c>
-      <c r="E80" s="7">
+      <c r="E80" s="2">
         <v>162</v>
       </c>
-      <c r="F80" s="7">
+      <c r="F80" s="2">
         <v>45023100</v>
       </c>
-      <c r="G80" s="7">
+      <c r="G80" s="2">
         <v>7</v>
       </c>
-      <c r="H80" s="8" t="s">
+      <c r="H80" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
-        <v>7501550</v>
-      </c>
-      <c r="B81" s="5" t="s">
+      <c r="A81" s="2">
+        <v>75015</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7">
+      <c r="C81" s="2"/>
+      <c r="D81" s="2">
         <v>100</v>
       </c>
-      <c r="E81" s="7">
+      <c r="E81" s="2">
         <v>254</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F81" s="2">
         <v>80160400</v>
       </c>
-      <c r="G81" s="7">
+      <c r="G81" s="2">
         <v>91</v>
       </c>
-      <c r="H81" s="8" t="s">
+      <c r="H81" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
-        <v>31193515</v>
-      </c>
-      <c r="B82" s="5" t="s">
+      <c r="A82" s="2">
+        <v>311935</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="7">
+      <c r="C82" s="2"/>
+      <c r="D82" s="2">
         <v>90</v>
       </c>
-      <c r="E82" s="7">
+      <c r="E82" s="2">
         <v>958.5</v>
       </c>
-      <c r="F82" s="7">
+      <c r="F82" s="2">
         <v>49033300</v>
       </c>
-      <c r="G82" s="7">
+      <c r="G82" s="2">
         <v>68</v>
       </c>
-      <c r="H82" s="8" t="s">
+      <c r="H82" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
-        <v>31323633</v>
-      </c>
-      <c r="B83" s="5" t="s">
+      <c r="A83" s="2">
+        <v>313236</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C83" s="6"/>
-      <c r="D83" s="7">
+      <c r="C83" s="2"/>
+      <c r="D83" s="2">
         <v>3</v>
       </c>
-      <c r="E83" s="7">
+      <c r="E83" s="2">
         <v>72.84</v>
       </c>
-      <c r="F83" s="7">
+      <c r="F83" s="2">
         <v>30085500</v>
       </c>
-      <c r="G83" s="7">
+      <c r="G83" s="2">
         <v>16</v>
       </c>
-      <c r="H83" s="8" t="s">
+      <c r="H83" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
-        <v>23594490</v>
-      </c>
-      <c r="B84" s="5" t="s">
+      <c r="A84" s="2">
+        <v>235944</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="7">
-        <v>10</v>
-      </c>
-      <c r="E84" s="7">
+      <c r="C84" s="2"/>
+      <c r="D84" s="2">
+        <v>10</v>
+      </c>
+      <c r="E84" s="2">
         <v>44</v>
       </c>
-      <c r="F84" s="7">
+      <c r="F84" s="2">
         <v>5250000</v>
       </c>
-      <c r="G84" s="13">
+      <c r="G84" s="4">
         <v>2376</v>
       </c>
-      <c r="H84" s="8" t="s">
+      <c r="H84" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
-        <v>5354518</v>
-      </c>
-      <c r="B85" s="5" t="s">
+      <c r="A85" s="2">
+        <v>53545</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="7">
+      <c r="C85" s="2"/>
+      <c r="D85" s="2">
         <v>100</v>
       </c>
-      <c r="E85" s="7">
+      <c r="E85" s="2">
         <v>668</v>
       </c>
-      <c r="F85" s="7">
+      <c r="F85" s="2">
         <v>21033300</v>
       </c>
-      <c r="G85" s="7">
+      <c r="G85" s="2">
         <v>200</v>
       </c>
-      <c r="H85" s="8" t="s">
+      <c r="H85" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
-        <v>31148041</v>
-      </c>
-      <c r="B86" s="5" t="s">
+      <c r="A86" s="2">
+        <v>311480</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="6"/>
-      <c r="D86" s="7">
+      <c r="C86" s="2"/>
+      <c r="D86" s="2">
         <v>12</v>
       </c>
-      <c r="E86" s="7">
+      <c r="E86" s="2">
         <v>156.47999999999999</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F86" s="2">
         <v>42023200</v>
       </c>
-      <c r="G86" s="7">
+      <c r="G86" s="2">
         <v>5</v>
       </c>
-      <c r="H86" s="8" t="s">
+      <c r="H86" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
-        <v>13925804</v>
-      </c>
-      <c r="B87" s="5" t="s">
+      <c r="A87" s="2">
+        <v>139258</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="7">
+      <c r="C87" s="2"/>
+      <c r="D87" s="2">
         <v>100</v>
       </c>
-      <c r="E87" s="7">
+      <c r="E87" s="2">
         <v>56</v>
       </c>
-      <c r="F87" s="7">
+      <c r="F87" s="2">
         <v>64022000</v>
       </c>
-      <c r="G87" s="7">
+      <c r="G87" s="2">
         <v>337</v>
       </c>
-      <c r="H87" s="8" t="s">
+      <c r="H87" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
-        <v>5354518</v>
-      </c>
-      <c r="B88" s="5" t="s">
+      <c r="A88" s="2">
+        <v>53545</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="7">
+      <c r="C88" s="2"/>
+      <c r="D88" s="2">
         <v>100</v>
       </c>
-      <c r="E88" s="7">
+      <c r="E88" s="2">
         <v>668</v>
       </c>
-      <c r="F88" s="7">
+      <c r="F88" s="2">
         <v>21033300</v>
       </c>
-      <c r="G88" s="7">
+      <c r="G88" s="2">
         <v>200</v>
       </c>
-      <c r="H88" s="8" t="s">
+      <c r="H88" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>29480007</v>
-      </c>
-      <c r="B89" s="5" t="s">
+      <c r="A89" s="2">
+        <v>294800</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="7">
+      <c r="C89" s="2"/>
+      <c r="D89" s="2">
         <v>5</v>
       </c>
-      <c r="E89" s="7">
+      <c r="E89" s="2">
         <v>58.85</v>
       </c>
-      <c r="F89" s="7">
+      <c r="F89" s="2">
         <v>60046300</v>
       </c>
-      <c r="G89" s="7">
+      <c r="G89" s="2">
         <v>0</v>
       </c>
-      <c r="H89" s="8" t="s">
+      <c r="H89" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
-        <v>21180889</v>
-      </c>
-      <c r="B90" s="5" t="s">
+      <c r="A90" s="2">
+        <v>211808</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="7">
+      <c r="C90" s="2"/>
+      <c r="D90" s="2">
         <v>50</v>
       </c>
-      <c r="E90" s="7">
+      <c r="E90" s="2">
         <v>263.5</v>
       </c>
-      <c r="F90" s="7">
+      <c r="F90" s="2">
         <v>69041100</v>
       </c>
-      <c r="G90" s="7">
+      <c r="G90" s="2">
         <v>0</v>
       </c>
-      <c r="H90" s="8" t="s">
+      <c r="H90" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
-        <v>32013024</v>
-      </c>
-      <c r="B91" s="5" t="s">
+      <c r="A91" s="2">
+        <v>320130</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="7">
+      <c r="C91" s="2"/>
+      <c r="D91" s="2">
         <v>12</v>
       </c>
-      <c r="E91" s="7">
+      <c r="E91" s="2">
         <v>159.36000000000001</v>
       </c>
-      <c r="F91" s="7">
+      <c r="F91" s="2">
         <v>63041200</v>
       </c>
-      <c r="G91" s="7">
+      <c r="G91" s="2">
         <v>38</v>
       </c>
-      <c r="H91" s="8" t="s">
+      <c r="H91" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
-        <v>13943660</v>
-      </c>
-      <c r="B92" s="5" t="s">
+      <c r="A92" s="2">
+        <v>139436</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="7">
+      <c r="C92" s="2"/>
+      <c r="D92" s="2">
         <v>12</v>
       </c>
-      <c r="E92" s="7">
+      <c r="E92" s="2">
         <v>83.4</v>
       </c>
-      <c r="F92" s="7">
+      <c r="F92" s="2">
         <v>30053200</v>
       </c>
-      <c r="G92" s="7">
+      <c r="G92" s="2">
         <v>2</v>
       </c>
-      <c r="H92" s="8" t="s">
+      <c r="H92" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
-        <v>21652779</v>
-      </c>
-      <c r="B93" s="5" t="s">
+      <c r="A93" s="2">
+        <v>216527</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="7">
+      <c r="C93" s="2"/>
+      <c r="D93" s="2">
         <v>6</v>
       </c>
-      <c r="E93" s="7">
+      <c r="E93" s="2">
         <v>275.52</v>
       </c>
-      <c r="F93" s="6"/>
-      <c r="G93" s="7">
+      <c r="F93" s="2"/>
+      <c r="G93" s="2">
         <v>0</v>
       </c>
-      <c r="H93" s="8" t="s">
+      <c r="H93" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
-        <v>3241974</v>
-      </c>
-      <c r="B94" s="5" t="s">
+      <c r="A94" s="2">
+        <v>32419</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="7">
-        <v>10</v>
-      </c>
-      <c r="E94" s="7">
+      <c r="C94" s="2"/>
+      <c r="D94" s="2">
+        <v>10</v>
+      </c>
+      <c r="E94" s="2">
         <v>26.5</v>
       </c>
-      <c r="F94" s="7">
+      <c r="F94" s="2">
         <v>16012300</v>
       </c>
-      <c r="G94" s="7">
+      <c r="G94" s="2">
         <v>67</v>
       </c>
-      <c r="H94" s="8" t="s">
+      <c r="H94" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
-        <v>24931422</v>
-      </c>
-      <c r="B95" s="5" t="s">
+      <c r="A95" s="2">
+        <v>249314</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C95" s="6"/>
-      <c r="D95" s="7">
+      <c r="C95" s="2"/>
+      <c r="D95" s="2">
         <v>810</v>
       </c>
-      <c r="E95" s="7">
+      <c r="E95" s="2">
         <v>955.8</v>
       </c>
-      <c r="F95" s="7">
+      <c r="F95" s="2">
         <v>62073200</v>
       </c>
-      <c r="G95" s="13">
+      <c r="G95" s="4">
         <v>8081</v>
       </c>
-      <c r="H95" s="8" t="s">
+      <c r="H95" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
-        <v>5320330</v>
-      </c>
-      <c r="B96" s="5" t="s">
+      <c r="A96" s="2">
+        <v>53203</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="13">
+      <c r="C96" s="2"/>
+      <c r="D96" s="4">
         <v>1800</v>
       </c>
-      <c r="E96" s="12">
+      <c r="E96" s="3">
         <v>2016</v>
       </c>
-      <c r="F96" s="7">
+      <c r="F96" s="2">
         <v>1270000</v>
       </c>
-      <c r="G96" s="13">
+      <c r="G96" s="4">
         <v>8541</v>
       </c>
-      <c r="H96" s="8" t="s">
+      <c r="H96" s="2" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>